<commit_message>
Updated Lowes_Database.xlsx & Wholesaler_Database.xlsx
</commit_message>
<xml_diff>
--- a/XX_Url/Ferguson_URL.xlsx
+++ b/XX_Url/Ferguson_URL.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://orgcorona-my.sharepoint.com/personal/jmonsalvo_corona_com_co/Documents/03_Proy_ID/03_MACHINE_LEARNING/01_Projects/11_Web_Scrapping/Pricing/00_Sprint/00_Scrapping_code/XX_Url/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://orgcorona-my.sharepoint.com/personal/jmonsalvo_corona_com_co/Documents/03_Proy_ID/03_MACHINE_LEARNING/01_Projects/11_Web_Scrapping/00_Scrapping_git/XX_Url/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="13_ncr:1_{ADD8D484-5C23-40E6-B751-62A63769F47D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8A4CBC2-4AC7-4BFB-B003-2FDEE3A126B5}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="13_ncr:1_{ADD8D484-5C23-40E6-B751-62A63769F47D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48718FE7-4D0F-4B57-981F-4B0BCF91DBCE}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1101,8 +1101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K5"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1314,8 +1314,9 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="L5" r:id="rId1" xr:uid="{1CC81736-04CD-4F75-9172-6893B9D63B0A}"/>
+    <hyperlink ref="L2" r:id="rId2" xr:uid="{DE41BE7D-AF90-41FC-B787-107DD22EDCFF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>